<commit_message>
Voila mon ami Reedom
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/BR/BRA0300_to_BRA0400.xlsx
+++ b/CR - Cost Report/BOM/BR/BRA0300_to_BRA0400.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Optimus_2019\STUF2019\CR - Cost Report\BOM\BR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dossiers\ECL\Cours\EPSA\Github 2019\CR - Cost Report\BOM\BR\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBFF7DD-AE75-483E-BA5F-E67175C4E96C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>System</t>
   </si>
@@ -57,16 +58,7 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Name of the part</t>
-  </si>
-  <si>
-    <t>m or b</t>
-  </si>
-  <si>
     <t>Short description of the part</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number </t>
   </si>
   <si>
     <r>
@@ -99,21 +91,6 @@
     <t>BR_03001</t>
   </si>
   <si>
-    <t>BR_03002</t>
-  </si>
-  <si>
-    <t>BR_03003</t>
-  </si>
-  <si>
-    <t>BR_03004</t>
-  </si>
-  <si>
-    <t>BR_03005</t>
-  </si>
-  <si>
-    <t>BR_03006</t>
-  </si>
-  <si>
     <t>BR_A0004</t>
   </si>
   <si>
@@ -123,22 +100,25 @@
     <t>BR_04002</t>
   </si>
   <si>
-    <t>BR_04003</t>
-  </si>
-  <si>
-    <t>BR_04004</t>
-  </si>
-  <si>
-    <t>BR_04005</t>
-  </si>
-  <si>
-    <t>BR_04006</t>
+    <t>Master Cylinder</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>Master Cylinder support</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Threaded aluminum part which support the bottom of the master cylinder</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -555,12 +535,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -583,7 +563,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -600,260 +580,89 @@
     </row>
     <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4">
+        <v>2</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>16</v>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>9</v>
+      <c r="F5" s="4">
+        <v>2</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="27" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>9</v>
+        <v>20</v>
+      </c>
+      <c r="F6" s="4">
+        <v>2</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>